<commit_message>
fixed width of time during auto
fixed width of time during auto
</commit_message>
<xml_diff>
--- a/UnderGraduate/AD矫正.xlsx
+++ b/UnderGraduate/AD矫正.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Control\UnderGraduate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBAA6178-4F86-41E6-AFA5-2BE702049B69}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852EFE25-AF66-423A-87CB-1A3758EB6C75}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59396E9F-CC40-49B9-B717-D87370D8730E}"/>
   </bookViews>
@@ -22,10 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -390,7 +386,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -412,20 +408,20 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>-9.8970000000000002</v>
+        <v>-8.9320000000000004</v>
       </c>
       <c r="B2">
         <v>-196</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E3" si="0">$C$3*A2+$D$3</f>
-        <v>-196</v>
+        <f t="shared" ref="E2" si="0">$C$3*A2+$D$3</f>
+        <v>-195.99999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A1-A2</f>
-        <v>17.585999999999999</v>
+        <v>16.621000000000002</v>
       </c>
       <c r="B3">
         <f>B1-B2</f>
@@ -433,11 +429,11 @@
       </c>
       <c r="C3">
         <f>B3/A3</f>
-        <v>13.218469236892984</v>
+        <v>13.985921424703687</v>
       </c>
       <c r="D3">
         <f>B1-C3*A1</f>
-        <v>-65.176809962470145</v>
+        <v>-71.077749834546637</v>
       </c>
     </row>
   </sheetData>

</xml_diff>